<commit_message>
hooks added for the clear storage
</commit_message>
<xml_diff>
--- a/data/recruiterList.xlsx
+++ b/data/recruiterList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sameer\Desktop\Linkedin Automation Testing Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129A26E7-E59A-4DE6-9E5A-3FDFA738A167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953FD088-1855-45E1-A4E8-4DC17E574396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Sameer  </t>
   </si>
@@ -40,15 +40,6 @@
   </si>
   <si>
     <t>City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swaroop </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rony </t>
-  </si>
-  <si>
-    <t>H</t>
   </si>
 </sst>
 </file>
@@ -366,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,19 +390,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>